<commit_message>
Inserimento dati in alcuni grafici
</commit_message>
<xml_diff>
--- a/DocumentazioneEsterna/PianoDiQualifica/res/ResocontoAttivitaDiVerifica/res/metriche/grafici/qualitàProdotto/qualitàProdotto.xlsx
+++ b/DocumentazioneEsterna/PianoDiQualifica/res/ResocontoAttivitaDiVerifica/res/metriche/grafici/qualitàProdotto/qualitàProdotto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Università\Terzo anno\SWE\Progetto\Documentazione\DocumentazioneEsterna\PianoDiQualifica\res\ResocontoAttivitaDiVerifica\res\metriche\grafici\qualitàProdotto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA2C09A1-BFAC-4FAA-85E1-30668D5E2DB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F50CB2-6294-4E94-9923-00018FBBB413}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E6A987FF-90E1-49FC-8E34-192DB323E80C}"/>
   </bookViews>
@@ -33,15 +33,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="72">
   <si>
     <t>Periodo</t>
   </si>
   <si>
     <t>Ottimale</t>
-  </si>
-  <si>
-    <t>A</t>
   </si>
   <si>
     <t>Completezza informazioni</t>
@@ -107,12 +104,6 @@
     <t>numero funzioni</t>
   </si>
   <si>
-    <t>Funzione</t>
-  </si>
-  <si>
-    <t>numero parametri</t>
-  </si>
-  <si>
     <t>SF</t>
   </si>
   <si>
@@ -123,6 +114,141 @@
   </si>
   <si>
     <t>Minuti</t>
+  </si>
+  <si>
+    <t>CartListSection</t>
+  </si>
+  <si>
+    <t>CartProductList</t>
+  </si>
+  <si>
+    <t>PayButton</t>
+  </si>
+  <si>
+    <t>PayButtonContent</t>
+  </si>
+  <si>
+    <t>CategoryList</t>
+  </si>
+  <si>
+    <t>CategoryListSection</t>
+  </si>
+  <si>
+    <t>DashboardLinks</t>
+  </si>
+  <si>
+    <t>ModifyProductForm</t>
+  </si>
+  <si>
+    <t>NewCategoryForm</t>
+  </si>
+  <si>
+    <t>NewProductForm</t>
+  </si>
+  <si>
+    <t>OldProductInformations</t>
+  </si>
+  <si>
+    <t>OrderList</t>
+  </si>
+  <si>
+    <t>OrderSection</t>
+  </si>
+  <si>
+    <t>ProductList</t>
+  </si>
+  <si>
+    <t>ProductSection</t>
+  </si>
+  <si>
+    <t>OrderDetails</t>
+  </si>
+  <si>
+    <t>CartSection</t>
+  </si>
+  <si>
+    <t>AddToCartList</t>
+  </si>
+  <si>
+    <t>CategoryProductList</t>
+  </si>
+  <si>
+    <t>ListingSection</t>
+  </si>
+  <si>
+    <t>ModifyProfileForm</t>
+  </si>
+  <si>
+    <t>ProfileButton</t>
+  </si>
+  <si>
+    <t>ProfileInfoForm</t>
+  </si>
+  <si>
+    <t>SearchBar</t>
+  </si>
+  <si>
+    <t>SearchBarSection</t>
+  </si>
+  <si>
+    <t>Fetcher</t>
+  </si>
+  <si>
+    <t>ModifyProducPage</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>OrderPage</t>
+  </si>
+  <si>
+    <t>ProducPage</t>
+  </si>
+  <si>
+    <t>ProductListingPage</t>
+  </si>
+  <si>
+    <t>EditProfile</t>
+  </si>
+  <si>
+    <t>ProfilePage</t>
+  </si>
+  <si>
+    <t>SearchPage</t>
+  </si>
+  <si>
+    <t>CategoryListHome</t>
+  </si>
+  <si>
+    <t>JustCreateProduct</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>ProductImage</t>
+  </si>
+  <si>
+    <t>ProductInCart</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>StoredProduct</t>
+  </si>
+  <si>
+    <t>Cart</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>User</t>
   </si>
 </sst>
 </file>
@@ -185,7 +311,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -208,11 +334,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -228,6 +365,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -2499,52 +2637,43 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Sviluppo!$C$137:$C$147</c:f>
+              <c:f>Sviluppo!$C$137:$C$144</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\-mm\-dd;@</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>44250</c:v>
+                  <c:v>44265</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44251</c:v>
+                  <c:v>44270</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44252</c:v>
+                  <c:v>44275</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44253</c:v>
+                  <c:v>44280</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44254</c:v>
+                  <c:v>44285</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44255</c:v>
+                  <c:v>44290</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44256</c:v>
+                  <c:v>44295</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44257</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44258</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>44259</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>44260</c:v>
+                  <c:v>44300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sviluppo!$F$137:$F$147</c:f>
+              <c:f>Sviluppo!$F$137:$F$144</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>15</c:v>
                 </c:pt>
@@ -2567,15 +2696,6 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
@@ -2629,52 +2749,43 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Sviluppo!$C$137:$C$147</c:f>
+              <c:f>Sviluppo!$C$137:$C$144</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\-mm\-dd;@</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>44250</c:v>
+                  <c:v>44265</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44251</c:v>
+                  <c:v>44270</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44252</c:v>
+                  <c:v>44275</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44253</c:v>
+                  <c:v>44280</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44254</c:v>
+                  <c:v>44285</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44255</c:v>
+                  <c:v>44290</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44256</c:v>
+                  <c:v>44295</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44257</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44258</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>44259</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>44260</c:v>
+                  <c:v>44300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sviluppo!$E$137:$E$147</c:f>
+              <c:f>Sviluppo!$E$137:$E$144</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -2697,15 +2808,6 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
@@ -2769,86 +2871,126 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sviluppo!$C$137:$C$147</c:f>
+              <c:f>Sviluppo!$C$137:$C$144</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\-mm\-dd;@</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>44250</c:v>
+                  <c:v>44265</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44251</c:v>
+                  <c:v>44270</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44252</c:v>
+                  <c:v>44275</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44253</c:v>
+                  <c:v>44280</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44254</c:v>
+                  <c:v>44285</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44255</c:v>
+                  <c:v>44290</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44256</c:v>
+                  <c:v>44295</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44257</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44258</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>44259</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>44260</c:v>
+                  <c:v>44300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sviluppo!$D$137:$D$147</c:f>
+              <c:f>Sviluppo!$D$137:$D$144</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>1.8181818181818181</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15</c:v>
+                  <c:v>1.6923076923076923</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>1.7333333333333334</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15</c:v>
+                  <c:v>1.6818181818181819</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15</c:v>
+                  <c:v>1.5714285714285714</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15</c:v>
+                  <c:v>1.5526315789473684</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15</c:v>
+                  <c:v>1.3777777777777778</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>15</c:v>
+                  <c:v>1.3777777777777778</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2977,6 +3119,8 @@
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
+        <c:majorUnit val="5"/>
+        <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
         <c:axId val="365909112"/>
@@ -3254,52 +3398,43 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Sviluppo!$C$187:$C$197</c:f>
+              <c:f>Sviluppo!$C$187:$C$194</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\-mm\-dd;@</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>44250</c:v>
+                  <c:v>44265</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44251</c:v>
+                  <c:v>44270</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44252</c:v>
+                  <c:v>44275</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44253</c:v>
+                  <c:v>44280</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44254</c:v>
+                  <c:v>44285</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44255</c:v>
+                  <c:v>44290</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44256</c:v>
+                  <c:v>44295</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44257</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44258</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>44259</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>44260</c:v>
+                  <c:v>44300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sviluppo!$F$187:$F$197</c:f>
+              <c:f>Sviluppo!$F$187:$F$194</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>15</c:v>
                 </c:pt>
@@ -3322,15 +3457,6 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
@@ -3384,52 +3510,43 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Sviluppo!$C$187:$C$197</c:f>
+              <c:f>Sviluppo!$C$187:$C$194</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\-mm\-dd;@</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>44250</c:v>
+                  <c:v>44265</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44251</c:v>
+                  <c:v>44270</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44252</c:v>
+                  <c:v>44275</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44253</c:v>
+                  <c:v>44280</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44254</c:v>
+                  <c:v>44285</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44255</c:v>
+                  <c:v>44290</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44256</c:v>
+                  <c:v>44295</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44257</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44258</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>44259</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>44260</c:v>
+                  <c:v>44300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sviluppo!$E$187:$E$197</c:f>
+              <c:f>Sviluppo!$E$187:$E$194</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -3452,15 +3569,6 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
@@ -3524,86 +3632,126 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sviluppo!$C$187:$C$197</c:f>
+              <c:f>Sviluppo!$C$187:$C$194</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\-mm\-dd;@</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>44250</c:v>
+                  <c:v>44265</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44251</c:v>
+                  <c:v>44270</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44252</c:v>
+                  <c:v>44275</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44253</c:v>
+                  <c:v>44280</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44254</c:v>
+                  <c:v>44285</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44255</c:v>
+                  <c:v>44290</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44256</c:v>
+                  <c:v>44295</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44257</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44258</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>44259</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>44260</c:v>
+                  <c:v>44300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sviluppo!$D$187:$D$197</c:f>
+              <c:f>Sviluppo!$D$187:$D$194</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>15</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3732,6 +3880,8 @@
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
+        <c:majorUnit val="5"/>
+        <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
         <c:axId val="365909112"/>
@@ -4009,52 +4159,43 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Sviluppo!$C$251:$C$261</c:f>
+              <c:f>Sviluppo!$C$251:$C$258</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\-mm\-dd;@</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>44250</c:v>
+                  <c:v>44265</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44251</c:v>
+                  <c:v>44270</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44252</c:v>
+                  <c:v>44275</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44253</c:v>
+                  <c:v>44280</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44254</c:v>
+                  <c:v>44285</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44255</c:v>
+                  <c:v>44290</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44256</c:v>
+                  <c:v>44295</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44257</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44258</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>44259</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>44260</c:v>
+                  <c:v>44300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sviluppo!$F$251:$F$261</c:f>
+              <c:f>Sviluppo!$F$251:$F$258</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>6</c:v>
                 </c:pt>
@@ -4077,15 +4218,6 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -4139,52 +4271,43 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Sviluppo!$C$251:$C$261</c:f>
+              <c:f>Sviluppo!$C$251:$C$258</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\-mm\-dd;@</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>44250</c:v>
+                  <c:v>44265</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44251</c:v>
+                  <c:v>44270</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44252</c:v>
+                  <c:v>44275</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44253</c:v>
+                  <c:v>44280</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44254</c:v>
+                  <c:v>44285</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44255</c:v>
+                  <c:v>44290</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44256</c:v>
+                  <c:v>44295</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44257</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44258</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>44259</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>44260</c:v>
+                  <c:v>44300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sviluppo!$E$251:$E$261</c:f>
+              <c:f>Sviluppo!$E$251:$E$258</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -4207,15 +4330,6 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
@@ -4279,86 +4393,126 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sviluppo!$C$251:$C$261</c:f>
+              <c:f>Sviluppo!$C$251:$C$258</c:f>
               <c:numCache>
                 <c:formatCode>yyyy\-mm\-dd;@</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>44250</c:v>
+                  <c:v>44265</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44251</c:v>
+                  <c:v>44270</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44252</c:v>
+                  <c:v>44275</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44253</c:v>
+                  <c:v>44280</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44254</c:v>
+                  <c:v>44285</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44255</c:v>
+                  <c:v>44290</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44256</c:v>
+                  <c:v>44295</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44257</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44258</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>44259</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>44260</c:v>
+                  <c:v>44300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sviluppo!$D$251:$D$261</c:f>
+              <c:f>Sviluppo!$D$251:$D$258</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>0.70588235294117652</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15</c:v>
+                  <c:v>1.2857142857142858</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>1.553191489361702</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15</c:v>
+                  <c:v>1.56</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15</c:v>
+                  <c:v>1.5535714285714286</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15</c:v>
+                  <c:v>1.5614035087719298</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15</c:v>
+                  <c:v>1.523076923076923</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>15</c:v>
+                  <c:v>1.5074626865671641</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4487,6 +4641,8 @@
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
+        <c:majorUnit val="5"/>
+        <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
         <c:axId val="365909112"/>
@@ -4769,37 +4925,28 @@
                 <c:formatCode>yyyy\-mm\-dd;@</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>44250</c:v>
+                  <c:v>44265</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44251</c:v>
+                  <c:v>44270</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44252</c:v>
+                  <c:v>44275</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44253</c:v>
+                  <c:v>44280</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44254</c:v>
+                  <c:v>44285</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44255</c:v>
+                  <c:v>44290</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44256</c:v>
+                  <c:v>44295</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44257</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44258</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>44259</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>44260</c:v>
+                  <c:v>44300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4832,15 +4979,6 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -4899,37 +5037,28 @@
                 <c:formatCode>yyyy\-mm\-dd;@</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>44250</c:v>
+                  <c:v>44265</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44251</c:v>
+                  <c:v>44270</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44252</c:v>
+                  <c:v>44275</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44253</c:v>
+                  <c:v>44280</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44254</c:v>
+                  <c:v>44285</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44255</c:v>
+                  <c:v>44290</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44256</c:v>
+                  <c:v>44295</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44257</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44258</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>44259</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>44260</c:v>
+                  <c:v>44300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4962,15 +5091,6 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
@@ -5034,6 +5154,64 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Sviluppo!$C$308:$C$318</c:f>
@@ -5041,37 +5219,28 @@
                 <c:formatCode>yyyy\-mm\-dd;@</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>44250</c:v>
+                  <c:v>44265</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44251</c:v>
+                  <c:v>44270</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44252</c:v>
+                  <c:v>44275</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44253</c:v>
+                  <c:v>44280</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44254</c:v>
+                  <c:v>44285</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44255</c:v>
+                  <c:v>44290</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44256</c:v>
+                  <c:v>44295</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44257</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>44258</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>44259</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>44260</c:v>
+                  <c:v>44300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5083,37 +5252,28 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>0.91304347826086951</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15</c:v>
+                  <c:v>1.0689655172413792</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>0.91666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15</c:v>
+                  <c:v>1.4098360655737705</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15</c:v>
+                  <c:v>1.4098360655737705</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15</c:v>
+                  <c:v>1.4098360655737705</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>15</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5242,6 +5402,8 @@
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
+        <c:majorUnit val="5"/>
+        <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
         <c:axId val="365909112"/>
@@ -10791,7 +10953,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>297480</xdr:colOff>
+      <xdr:colOff>68580</xdr:colOff>
       <xdr:row>175</xdr:row>
       <xdr:rowOff>156960</xdr:rowOff>
     </xdr:to>
@@ -10828,8 +10990,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>297480</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1554480</xdr:colOff>
       <xdr:row>223</xdr:row>
       <xdr:rowOff>156960</xdr:rowOff>
     </xdr:to>
@@ -10867,7 +11029,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>297480</xdr:colOff>
+      <xdr:colOff>22860</xdr:colOff>
       <xdr:row>290</xdr:row>
       <xdr:rowOff>156960</xdr:rowOff>
     </xdr:to>
@@ -10905,7 +11067,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>373680</xdr:colOff>
+      <xdr:colOff>60960</xdr:colOff>
       <xdr:row>349</xdr:row>
       <xdr:rowOff>73140</xdr:rowOff>
     </xdr:to>
@@ -11272,10 +11434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B4F4DE7-87B1-4CD4-B318-8D739C70AC78}">
-  <dimension ref="C6:K379"/>
+  <dimension ref="C6:L379"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B64" workbookViewId="0">
-      <selection activeCell="J53" sqref="J53"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="G343" sqref="G343"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11283,15 +11445,16 @@
     <col min="3" max="3" width="37" customWidth="1"/>
     <col min="6" max="6" width="23.6640625" customWidth="1"/>
     <col min="7" max="7" width="24.77734375" customWidth="1"/>
-    <col min="8" max="8" width="18.88671875" customWidth="1"/>
+    <col min="8" max="8" width="22.5546875" customWidth="1"/>
     <col min="9" max="9" width="16.88671875" customWidth="1"/>
     <col min="10" max="10" width="14.33203125" customWidth="1"/>
     <col min="11" max="11" width="18.77734375" customWidth="1"/>
+    <col min="12" max="12" width="16.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C6" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -11302,16 +11465,16 @@
         <v>0</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>1</v>
       </c>
       <c r="F7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>5</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>6</v>
       </c>
       <c r="H7" s="7"/>
     </row>
@@ -11358,7 +11521,7 @@
         <v>44275</v>
       </c>
       <c r="D10" s="6">
-        <f t="shared" ref="D10:D18" si="0">(1-F10/G10)</f>
+        <f t="shared" ref="D10:D15" si="0">(1-F10/G10)</f>
         <v>0.53</v>
       </c>
       <c r="E10" s="6">
@@ -11486,7 +11649,7 @@
     </row>
     <row r="44" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C44" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -11497,19 +11660,19 @@
         <v>0</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>1</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G45" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H45" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="H45" s="5" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="46" spans="3:8" x14ac:dyDescent="0.3">
@@ -11538,7 +11701,7 @@
         <v>44270</v>
       </c>
       <c r="D47" s="6">
-        <f t="shared" ref="D47:D56" si="1">(G47/H47)</f>
+        <f t="shared" ref="D47:D53" si="1">(G47/H47)</f>
         <v>0.1</v>
       </c>
       <c r="E47" s="6">
@@ -11706,7 +11869,7 @@
     </row>
     <row r="88" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C88" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
@@ -11717,13 +11880,13 @@
         <v>0</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E89" s="5" t="s">
         <v>1</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G89" s="7"/>
       <c r="H89" s="7"/>
@@ -11906,7 +12069,7 @@
     </row>
     <row r="135" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C135" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D135" s="2"/>
       <c r="E135" s="2"/>
@@ -11916,28 +12079,28 @@
         <v>0</v>
       </c>
       <c r="D136" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E136" s="5" t="s">
         <v>1</v>
       </c>
       <c r="F136" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G136" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H136" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="H136" s="5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="137" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C137" s="10">
-        <v>44250</v>
+        <v>44265</v>
       </c>
       <c r="D137" s="9">
         <f>G137/H137</f>
-        <v>15</v>
+        <v>1.8181818181818181</v>
       </c>
       <c r="E137" s="9">
         <v>10</v>
@@ -11946,21 +12109,21 @@
         <v>15</v>
       </c>
       <c r="G137" s="9">
-        <f>G138</f>
-        <v>165</v>
+        <f>SUM(L161:L171)</f>
+        <v>20</v>
       </c>
       <c r="H137" s="9">
-        <f>COUNTA(H161:H171)</f>
+        <f>COUNTA(K161:K171)</f>
         <v>11</v>
       </c>
     </row>
     <row r="138" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C138" s="10">
-        <v>44251</v>
+        <v>44270</v>
       </c>
       <c r="D138" s="9">
         <f t="shared" ref="D138:D147" si="2">G138/H138</f>
-        <v>15</v>
+        <v>1.6923076923076923</v>
       </c>
       <c r="E138" s="9">
         <v>10</v>
@@ -11969,21 +12132,21 @@
         <v>15</v>
       </c>
       <c r="G138" s="9">
-        <f>SUM(I161:I171)</f>
-        <v>165</v>
+        <f>SUM(L161:L173)</f>
+        <v>22</v>
       </c>
       <c r="H138" s="9">
-        <f>COUNTA(H161:H171)</f>
-        <v>11</v>
+        <f>COUNTA(K161:K173)</f>
+        <v>13</v>
       </c>
     </row>
     <row r="139" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C139" s="10">
-        <v>44252</v>
+        <v>44275</v>
       </c>
       <c r="D139" s="9">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>1.7333333333333334</v>
       </c>
       <c r="E139" s="9">
         <v>10</v>
@@ -11992,21 +12155,21 @@
         <v>15</v>
       </c>
       <c r="G139" s="9">
-        <f>SUM(I161:I171)</f>
-        <v>165</v>
+        <f>SUM(L161:L175)</f>
+        <v>26</v>
       </c>
       <c r="H139" s="9">
-        <f>COUNTA(H161:H171)</f>
-        <v>11</v>
+        <f>COUNTA(K161:K175)</f>
+        <v>15</v>
       </c>
     </row>
     <row r="140" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C140" s="10">
-        <v>44253</v>
+        <v>44280</v>
       </c>
       <c r="D140" s="9">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>1.6818181818181819</v>
       </c>
       <c r="E140" s="9">
         <v>10</v>
@@ -12015,21 +12178,21 @@
         <v>15</v>
       </c>
       <c r="G140" s="9">
-        <f>SUM(I161:I171)</f>
-        <v>165</v>
+        <f>SUM(L161:L182)</f>
+        <v>37</v>
       </c>
       <c r="H140" s="9">
-        <f>COUNTA(H161:H171)</f>
-        <v>11</v>
+        <f>COUNTA(K161:K182)</f>
+        <v>22</v>
       </c>
     </row>
     <row r="141" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C141" s="10">
-        <v>44254</v>
+        <v>44285</v>
       </c>
       <c r="D141" s="9">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>1.5714285714285714</v>
       </c>
       <c r="E141" s="9">
         <v>10</v>
@@ -12038,21 +12201,21 @@
         <v>15</v>
       </c>
       <c r="G141" s="9">
-        <f>SUM(I161:I171)</f>
-        <v>165</v>
+        <f>SUM(L161:L195)</f>
+        <v>55</v>
       </c>
       <c r="H141" s="9">
-        <f>COUNTA(H161:H171)</f>
-        <v>11</v>
+        <f>COUNTA(K161:K195)</f>
+        <v>35</v>
       </c>
     </row>
     <row r="142" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C142" s="10">
-        <v>44255</v>
+        <v>44290</v>
       </c>
       <c r="D142" s="9">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>1.5526315789473684</v>
       </c>
       <c r="E142" s="9">
         <v>10</v>
@@ -12061,21 +12224,21 @@
         <v>15</v>
       </c>
       <c r="G142" s="9">
-        <f>SUM(I161:I171)</f>
-        <v>165</v>
+        <f>SUM(L161:L198)</f>
+        <v>59</v>
       </c>
       <c r="H142" s="9">
-        <f>COUNTA(H161:H171)</f>
-        <v>11</v>
+        <f>COUNTA(K161:K198)</f>
+        <v>38</v>
       </c>
     </row>
     <row r="143" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C143" s="10">
-        <v>44256</v>
+        <v>44295</v>
       </c>
       <c r="D143" s="9">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>1.3777777777777778</v>
       </c>
       <c r="E143" s="9">
         <v>10</v>
@@ -12084,21 +12247,21 @@
         <v>15</v>
       </c>
       <c r="G143" s="9">
-        <f>SUM(I161:I171)</f>
-        <v>165</v>
+        <f>SUM(L161:L205)</f>
+        <v>62</v>
       </c>
       <c r="H143" s="9">
-        <f>COUNTA(H161:H171)</f>
-        <v>11</v>
+        <f>COUNTA(K161:K205)</f>
+        <v>45</v>
       </c>
     </row>
     <row r="144" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C144" s="10">
-        <v>44257</v>
+        <v>44300</v>
       </c>
       <c r="D144" s="9">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>1.3777777777777778</v>
       </c>
       <c r="E144" s="9">
         <v>10</v>
@@ -12107,213 +12270,284 @@
         <v>15</v>
       </c>
       <c r="G144" s="9">
-        <f>SUM(I161:I171)</f>
-        <v>165</v>
+        <f>SUM(L161:L205)</f>
+        <v>62</v>
       </c>
       <c r="H144" s="9">
-        <f>COUNTA(H161:H171)</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="145" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C145" s="10">
-        <v>44258</v>
-      </c>
-      <c r="D145" s="9">
-        <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="E145" s="9">
-        <v>10</v>
-      </c>
-      <c r="F145" s="9">
-        <v>15</v>
-      </c>
-      <c r="G145" s="9">
-        <f>SUM(I161:I171)</f>
-        <v>165</v>
-      </c>
-      <c r="H145" s="9">
-        <f>COUNTA(H161:H171)</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="146" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C146" s="10">
-        <v>44259</v>
-      </c>
-      <c r="D146" s="9">
-        <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="E146" s="9">
-        <v>10</v>
-      </c>
-      <c r="F146" s="9">
-        <v>15</v>
-      </c>
-      <c r="G146" s="9">
-        <f>SUM(I161:I171)</f>
-        <v>165</v>
-      </c>
-      <c r="H146" s="9">
-        <f>COUNTA(H161:H171)</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="147" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C147" s="10">
-        <v>44260</v>
-      </c>
-      <c r="D147" s="9">
-        <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="E147" s="9">
-        <v>10</v>
-      </c>
-      <c r="F147" s="9">
-        <v>15</v>
-      </c>
-      <c r="G147" s="9">
-        <f>SUM(I161:I171)</f>
-        <v>165</v>
-      </c>
-      <c r="H147" s="9">
-        <f>COUNTA(H161:H171)</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="160" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="H160" s="5" t="s">
+        <f>COUNTA(K161:K205)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="145" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C145" s="10"/>
+      <c r="D145" s="9"/>
+      <c r="E145" s="9"/>
+      <c r="F145" s="9"/>
+      <c r="G145" s="9"/>
+      <c r="H145" s="9"/>
+    </row>
+    <row r="146" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C146" s="10"/>
+      <c r="D146" s="9"/>
+      <c r="E146" s="9"/>
+      <c r="F146" s="9"/>
+      <c r="G146" s="9"/>
+      <c r="H146" s="9"/>
+    </row>
+    <row r="147" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C147" s="10"/>
+      <c r="D147" s="9"/>
+      <c r="E147" s="9"/>
+      <c r="F147" s="9"/>
+      <c r="G147" s="9"/>
+      <c r="H147" s="9"/>
+    </row>
+    <row r="160" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="K160" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L160" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I160" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="161" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="H161" s="9" t="s">
+    </row>
+    <row r="161" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K161" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="L161" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="162" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K162" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L162" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K163" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="L163" s="9">
         <v>2</v>
       </c>
-      <c r="I161" s="9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="162" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="H162" s="9" t="s">
+    </row>
+    <row r="164" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K164" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="L164" s="9">
         <v>2</v>
       </c>
-      <c r="I162" s="9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="163" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="H163" s="9" t="s">
+    </row>
+    <row r="165" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K165" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L165" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K166" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="L166" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="167" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K167" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="L167" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K168" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="L168" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K169" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="L169" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K170" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="L170" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K171" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="L171" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K172" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="L172" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K173" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="L173" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K174" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="L174" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K175" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="L175" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="176" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K176" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="L176" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="K177" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="L177" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="K178" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="L178" s="15">
         <v>2</v>
       </c>
-      <c r="I163" s="9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="164" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="H164" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="I164" s="9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="165" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="H165" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="I165" s="9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="166" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="H166" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="I166" s="9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="167" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="H167" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="I167" s="9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="168" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="H168" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="I168" s="9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="169" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="H169" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="I169" s="9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="170" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="H170" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="I170" s="9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="171" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="H171" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="I171" s="9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="185" spans="3:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="179" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="K179" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="L179" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="K180" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="L180" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="K181" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="L181" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="K182" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="L182" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="183" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="K183" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="L183" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="K184" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="L184" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C185" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D185" s="2"/>
       <c r="E185" s="2"/>
-    </row>
-    <row r="186" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="K185" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="L185" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C186" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D186" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E186" s="5" t="s">
         <v>1</v>
       </c>
       <c r="F186" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G186" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H186" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H186" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="187" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="K186" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="L186" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C187" s="10">
-        <v>44250</v>
+        <v>44265</v>
       </c>
       <c r="D187" s="9">
         <f>G187/H187</f>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E187" s="9">
         <v>10</v>
@@ -12322,21 +12556,27 @@
         <v>15</v>
       </c>
       <c r="G187" s="9">
-        <f>SUM(I206:I216)</f>
-        <v>165</v>
+        <f>SUM(L210)</f>
+        <v>11</v>
       </c>
       <c r="H187" s="9">
-        <f>COUNTA(H206:H216)</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="188" spans="3:8" x14ac:dyDescent="0.3">
+        <f>COUNTA(K210)</f>
+        <v>1</v>
+      </c>
+      <c r="K187" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="L187" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C188" s="10">
-        <v>44251</v>
+        <v>44270</v>
       </c>
       <c r="D188" s="9">
         <f t="shared" ref="D188:D197" si="3">G188/H188</f>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E188" s="9">
         <v>10</v>
@@ -12345,21 +12585,27 @@
         <v>15</v>
       </c>
       <c r="G188" s="9">
-        <f>SUM(I206:I216)</f>
-        <v>165</v>
+        <f>SUM(L210)</f>
+        <v>11</v>
       </c>
       <c r="H188" s="9">
-        <f>COUNTA(H161:H171)</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="189" spans="3:8" x14ac:dyDescent="0.3">
+        <f>COUNTA(K210)</f>
+        <v>1</v>
+      </c>
+      <c r="K188" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="L188" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="189" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C189" s="10">
-        <v>44252</v>
+        <v>44275</v>
       </c>
       <c r="D189" s="9">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>6.5</v>
       </c>
       <c r="E189" s="9">
         <v>10</v>
@@ -12368,21 +12614,27 @@
         <v>15</v>
       </c>
       <c r="G189" s="9">
-        <f>SUM(I206:I216)</f>
-        <v>165</v>
+        <f>SUM(L210:L211)</f>
+        <v>13</v>
       </c>
       <c r="H189" s="9">
-        <f>COUNTA(H161:H171)</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="190" spans="3:8" x14ac:dyDescent="0.3">
+        <f>COUNTA(K210:K211)</f>
+        <v>2</v>
+      </c>
+      <c r="K189" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="L189" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C190" s="10">
-        <v>44253</v>
+        <v>44280</v>
       </c>
       <c r="D190" s="9">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E190" s="9">
         <v>10</v>
@@ -12391,21 +12643,27 @@
         <v>15</v>
       </c>
       <c r="G190" s="9">
-        <f>SUM(I206:I216)</f>
-        <v>165</v>
+        <f>SUM(L210:L212)</f>
+        <v>15</v>
       </c>
       <c r="H190" s="9">
-        <f>COUNTA(H161:H171)</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="191" spans="3:8" x14ac:dyDescent="0.3">
+        <f>COUNTA(L210:L212)</f>
+        <v>3</v>
+      </c>
+      <c r="K190" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="L190" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="191" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C191" s="10">
-        <v>44254</v>
+        <v>44285</v>
       </c>
       <c r="D191" s="9">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E191" s="9">
         <v>10</v>
@@ -12414,21 +12672,27 @@
         <v>15</v>
       </c>
       <c r="G191" s="9">
-        <f>SUM(I206:I216)</f>
-        <v>165</v>
+        <f>SUM(L210:L212)</f>
+        <v>15</v>
       </c>
       <c r="H191" s="9">
-        <f>COUNTA(H161:H171)</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="192" spans="3:8" x14ac:dyDescent="0.3">
+        <f>COUNTA(L210:L212)</f>
+        <v>3</v>
+      </c>
+      <c r="K191" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="L191" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="192" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C192" s="10">
-        <v>44255</v>
+        <v>44290</v>
       </c>
       <c r="D192" s="9">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E192" s="9">
         <v>10</v>
@@ -12437,21 +12701,27 @@
         <v>15</v>
       </c>
       <c r="G192" s="9">
-        <f>SUM(I206:I216)</f>
-        <v>165</v>
+        <f>SUM(L210:L212)</f>
+        <v>15</v>
       </c>
       <c r="H192" s="9">
-        <f>COUNTA(H161:H171)</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="193" spans="3:9" x14ac:dyDescent="0.3">
+        <f>COUNTA(K210:K212)</f>
+        <v>3</v>
+      </c>
+      <c r="K192" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="L192" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C193" s="10">
-        <v>44256</v>
+        <v>44295</v>
       </c>
       <c r="D193" s="9">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E193" s="9">
         <v>10</v>
@@ -12460,21 +12730,27 @@
         <v>15</v>
       </c>
       <c r="G193" s="9">
-        <f>SUM(I206:I216)</f>
-        <v>165</v>
+        <f>SUM(L210:L214)</f>
+        <v>20</v>
       </c>
       <c r="H193" s="9">
-        <f>COUNTA(H161:H171)</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="194" spans="3:9" x14ac:dyDescent="0.3">
+        <f>COUNTA(K210:K214)</f>
+        <v>5</v>
+      </c>
+      <c r="K193" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="L193" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C194" s="10">
-        <v>44257</v>
+        <v>44300</v>
       </c>
       <c r="D194" s="9">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E194" s="9">
         <v>10</v>
@@ -12483,182 +12759,201 @@
         <v>15</v>
       </c>
       <c r="G194" s="9">
-        <f>SUM(I206:I216)</f>
-        <v>165</v>
+        <f>SUM(L210:L214)</f>
+        <v>20</v>
       </c>
       <c r="H194" s="9">
-        <f>COUNTA(H161:H171)</f>
+        <f>COUNTA(K210:K214)</f>
+        <v>5</v>
+      </c>
+      <c r="K194" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="L194" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C195" s="10"/>
+      <c r="D195" s="9"/>
+      <c r="E195" s="9"/>
+      <c r="F195" s="9"/>
+      <c r="G195" s="9"/>
+      <c r="H195" s="9"/>
+      <c r="K195" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="L195" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="196" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C196" s="10"/>
+      <c r="D196" s="9"/>
+      <c r="E196" s="9"/>
+      <c r="F196" s="9"/>
+      <c r="G196" s="9"/>
+      <c r="H196" s="9"/>
+      <c r="K196" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="L196" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C197" s="10"/>
+      <c r="D197" s="9"/>
+      <c r="E197" s="9"/>
+      <c r="F197" s="9"/>
+      <c r="G197" s="9"/>
+      <c r="H197" s="9"/>
+      <c r="K197" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="L197" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="198" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="K198" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="L198" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="K199" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="L199" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="K200" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="L200" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="K201" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="L201" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="K202" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="L202" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="K203" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="L203" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="204" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="K204" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="L204" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="K205" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="L205" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K209" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L209" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="210" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K210" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="L210" s="9">
         <v>11</v>
       </c>
     </row>
-    <row r="195" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C195" s="10">
-        <v>44258</v>
-      </c>
-      <c r="D195" s="9">
-        <f t="shared" si="3"/>
-        <v>15</v>
-      </c>
-      <c r="E195" s="9">
-        <v>10</v>
-      </c>
-      <c r="F195" s="9">
-        <v>15</v>
-      </c>
-      <c r="G195" s="9">
-        <f>SUM(I206:I216)</f>
-        <v>165</v>
-      </c>
-      <c r="H195" s="9">
-        <f>COUNTA(H161:H171)</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="196" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C196" s="10">
-        <v>44259</v>
-      </c>
-      <c r="D196" s="9">
-        <f t="shared" si="3"/>
-        <v>15</v>
-      </c>
-      <c r="E196" s="9">
-        <v>10</v>
-      </c>
-      <c r="F196" s="9">
-        <v>15</v>
-      </c>
-      <c r="G196" s="9">
-        <f>SUM(I206:I216)</f>
-        <v>165</v>
-      </c>
-      <c r="H196" s="9">
-        <f>COUNTA(H161:H171)</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="197" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C197" s="10">
-        <v>44260</v>
-      </c>
-      <c r="D197" s="9">
-        <f t="shared" si="3"/>
-        <v>15</v>
-      </c>
-      <c r="E197" s="9">
-        <v>10</v>
-      </c>
-      <c r="F197" s="9">
-        <v>15</v>
-      </c>
-      <c r="G197" s="9">
-        <f>SUM(I206:I216)</f>
-        <v>165</v>
-      </c>
-      <c r="H197" s="9">
-        <f>COUNTA(H161:H171)</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="205" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="H205" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I205" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="206" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="H206" s="9" t="s">
+    <row r="211" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K211" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="L211" s="9">
         <v>2</v>
       </c>
-      <c r="I206" s="9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="207" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="H207" s="9" t="s">
+    </row>
+    <row r="212" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K212" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="L212" s="9">
         <v>2</v>
       </c>
-      <c r="I207" s="9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="208" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="H208" s="9" t="s">
+    </row>
+    <row r="213" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K213" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="L213" s="9">
         <v>2</v>
       </c>
-      <c r="I208" s="9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="209" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="H209" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="I209" s="9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="210" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="H210" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="I210" s="9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="211" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="H211" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="I211" s="9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="212" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="H212" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="I212" s="9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="213" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="H213" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="I213" s="9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="214" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="H214" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="I214" s="9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="215" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="H215" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="I215" s="9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="216" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="H216" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="I216" s="9">
-        <v>15</v>
-      </c>
+    </row>
+    <row r="214" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K214" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="L214" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="215" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K215" s="9"/>
+      <c r="L215" s="9"/>
+    </row>
+    <row r="216" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K216" s="9"/>
+      <c r="L216" s="9"/>
+    </row>
+    <row r="217" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K217" s="9"/>
+      <c r="L217" s="9"/>
+    </row>
+    <row r="218" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K218" s="9"/>
+      <c r="L218" s="9"/>
+    </row>
+    <row r="219" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K219" s="9"/>
+      <c r="L219" s="9"/>
+    </row>
+    <row r="220" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K220" s="9"/>
+      <c r="L220" s="9"/>
     </row>
     <row r="249" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C249" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D249" s="2"/>
       <c r="E249" s="2"/>
@@ -12668,34 +12963,30 @@
         <v>0</v>
       </c>
       <c r="D250" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E250" s="5" t="s">
         <v>1</v>
       </c>
       <c r="F250" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G250" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H250" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H250" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J250" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="K250" s="5" t="s">
-        <v>25</v>
-      </c>
+      <c r="J250" s="7"/>
+      <c r="K250" s="7"/>
     </row>
     <row r="251" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C251" s="10">
-        <v>44250</v>
+        <v>44265</v>
       </c>
       <c r="D251" s="9">
         <f>G251/H251</f>
-        <v>15</v>
+        <v>0.70588235294117652</v>
       </c>
       <c r="E251" s="9">
         <v>3</v>
@@ -12704,27 +12995,21 @@
         <v>6</v>
       </c>
       <c r="G251" s="9">
-        <f>SUM(K251:K261)</f>
-        <v>165</v>
+        <v>12</v>
       </c>
       <c r="H251" s="9">
-        <f>COUNTA(J251:J261)</f>
-        <v>11</v>
-      </c>
-      <c r="J251" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="K251" s="9">
-        <v>15</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="J251" s="11"/>
+      <c r="K251" s="11"/>
     </row>
     <row r="252" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C252" s="10">
-        <v>44251</v>
+        <v>44270</v>
       </c>
       <c r="D252" s="9">
         <f t="shared" ref="D252:D261" si="4">G252/H252</f>
-        <v>15</v>
+        <v>1.2857142857142858</v>
       </c>
       <c r="E252" s="9">
         <v>3</v>
@@ -12733,27 +13018,21 @@
         <v>6</v>
       </c>
       <c r="G252" s="9">
-        <f>SUM(K251:K261)</f>
-        <v>165</v>
+        <v>36</v>
       </c>
       <c r="H252" s="9">
-        <f>COUNTA(J251:J261)</f>
-        <v>11</v>
-      </c>
-      <c r="J252" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="K252" s="9">
-        <v>15</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="J252" s="11"/>
+      <c r="K252" s="11"/>
     </row>
     <row r="253" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C253" s="10">
-        <v>44252</v>
+        <v>44275</v>
       </c>
       <c r="D253" s="9">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>1.553191489361702</v>
       </c>
       <c r="E253" s="9">
         <v>3</v>
@@ -12762,27 +13041,23 @@
         <v>6</v>
       </c>
       <c r="G253" s="9">
-        <f>SUM(K251:K261)</f>
-        <v>165</v>
+        <f>37+36</f>
+        <v>73</v>
       </c>
       <c r="H253" s="9">
-        <f>COUNTA(J251:J261)</f>
-        <v>11</v>
-      </c>
-      <c r="J253" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="K253" s="9">
-        <v>15</v>
-      </c>
+        <f>19+28</f>
+        <v>47</v>
+      </c>
+      <c r="J253" s="11"/>
+      <c r="K253" s="11"/>
     </row>
     <row r="254" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C254" s="10">
-        <v>44253</v>
+        <v>44280</v>
       </c>
       <c r="D254" s="9">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>1.56</v>
       </c>
       <c r="E254" s="9">
         <v>3</v>
@@ -12791,27 +13066,23 @@
         <v>6</v>
       </c>
       <c r="G254" s="9">
-        <f>SUM(K251:K261)</f>
-        <v>165</v>
+        <f>78</f>
+        <v>78</v>
       </c>
       <c r="H254" s="9">
-        <f>COUNTA(J251:J261)</f>
-        <v>11</v>
-      </c>
-      <c r="J254" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="K254" s="9">
-        <v>15</v>
-      </c>
+        <f>50</f>
+        <v>50</v>
+      </c>
+      <c r="J254" s="11"/>
+      <c r="K254" s="11"/>
     </row>
     <row r="255" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C255" s="10">
-        <v>44254</v>
+        <v>44285</v>
       </c>
       <c r="D255" s="9">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>1.5535714285714286</v>
       </c>
       <c r="E255" s="9">
         <v>3</v>
@@ -12820,27 +13091,23 @@
         <v>6</v>
       </c>
       <c r="G255" s="9">
-        <f>SUM(K251:K261)</f>
-        <v>165</v>
+        <f>78+9</f>
+        <v>87</v>
       </c>
       <c r="H255" s="9">
-        <f>COUNTA(J251:J261)</f>
-        <v>11</v>
-      </c>
-      <c r="J255" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="K255" s="9">
-        <v>15</v>
-      </c>
+        <f>56</f>
+        <v>56</v>
+      </c>
+      <c r="J255" s="11"/>
+      <c r="K255" s="11"/>
     </row>
     <row r="256" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C256" s="10">
-        <v>44255</v>
+        <v>44290</v>
       </c>
       <c r="D256" s="9">
         <f>G256/H256</f>
-        <v>15</v>
+        <v>1.5614035087719298</v>
       </c>
       <c r="E256" s="9">
         <v>3</v>
@@ -12849,27 +13116,23 @@
         <v>6</v>
       </c>
       <c r="G256" s="9">
-        <f>SUM(K251:K261)</f>
-        <v>165</v>
+        <f>89</f>
+        <v>89</v>
       </c>
       <c r="H256" s="9">
-        <f>COUNTA(J251:J261)</f>
-        <v>11</v>
-      </c>
-      <c r="J256" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="K256" s="9">
-        <v>15</v>
-      </c>
+        <f>57</f>
+        <v>57</v>
+      </c>
+      <c r="J256" s="11"/>
+      <c r="K256" s="11"/>
     </row>
     <row r="257" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C257" s="10">
-        <v>44256</v>
+        <v>44295</v>
       </c>
       <c r="D257" s="9">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>1.523076923076923</v>
       </c>
       <c r="E257" s="9">
         <v>3</v>
@@ -12878,27 +13141,23 @@
         <v>6</v>
       </c>
       <c r="G257" s="9">
-        <f>SUM(K251:K261)</f>
-        <v>165</v>
+        <f>99</f>
+        <v>99</v>
       </c>
       <c r="H257" s="9">
-        <f>COUNTA(J251:J261)</f>
-        <v>11</v>
-      </c>
-      <c r="J257" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="K257" s="9">
-        <v>15</v>
-      </c>
+        <f>57+8</f>
+        <v>65</v>
+      </c>
+      <c r="J257" s="11"/>
+      <c r="K257" s="11"/>
     </row>
     <row r="258" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C258" s="10">
-        <v>44257</v>
+        <v>44300</v>
       </c>
       <c r="D258" s="9">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>1.5074626865671641</v>
       </c>
       <c r="E258" s="9">
         <v>3</v>
@@ -12907,110 +13166,49 @@
         <v>6</v>
       </c>
       <c r="G258" s="9">
-        <f>SUM(K251:K261)</f>
-        <v>165</v>
+        <f>101</f>
+        <v>101</v>
       </c>
       <c r="H258" s="9">
-        <f>COUNTA(J251:J261)</f>
-        <v>11</v>
-      </c>
-      <c r="J258" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="K258" s="9">
-        <v>15</v>
-      </c>
+        <f>67</f>
+        <v>67</v>
+      </c>
+      <c r="J258" s="11"/>
+      <c r="K258" s="11"/>
     </row>
     <row r="259" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C259" s="10">
-        <v>44258</v>
-      </c>
-      <c r="D259" s="9">
-        <f t="shared" si="4"/>
-        <v>15</v>
-      </c>
-      <c r="E259" s="9">
-        <v>3</v>
-      </c>
-      <c r="F259" s="9">
-        <v>6</v>
-      </c>
-      <c r="G259" s="9">
-        <f>SUM(K251:K261)</f>
-        <v>165</v>
-      </c>
-      <c r="H259" s="9">
-        <f>COUNTA(J251:J261)</f>
-        <v>11</v>
-      </c>
-      <c r="J259" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="K259" s="9">
-        <v>15</v>
-      </c>
+      <c r="C259" s="10"/>
+      <c r="D259" s="9"/>
+      <c r="E259" s="9"/>
+      <c r="F259" s="9"/>
+      <c r="G259" s="9"/>
+      <c r="H259" s="9"/>
+      <c r="J259" s="11"/>
+      <c r="K259" s="11"/>
     </row>
     <row r="260" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C260" s="10">
-        <v>44259</v>
-      </c>
-      <c r="D260" s="9">
-        <f t="shared" si="4"/>
-        <v>15</v>
-      </c>
-      <c r="E260" s="9">
-        <v>3</v>
-      </c>
-      <c r="F260" s="9">
-        <v>6</v>
-      </c>
-      <c r="G260" s="9">
-        <f>SUM(K251:K261)</f>
-        <v>165</v>
-      </c>
-      <c r="H260" s="9">
-        <f>COUNTA(J251:J261)</f>
-        <v>11</v>
-      </c>
-      <c r="J260" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="K260" s="9">
-        <v>15</v>
-      </c>
+      <c r="C260" s="10"/>
+      <c r="D260" s="9"/>
+      <c r="E260" s="9"/>
+      <c r="F260" s="9"/>
+      <c r="G260" s="9"/>
+      <c r="H260" s="9"/>
+      <c r="J260" s="11"/>
+      <c r="K260" s="11"/>
     </row>
     <row r="261" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C261" s="10">
-        <v>44260</v>
-      </c>
-      <c r="D261" s="9">
-        <f t="shared" si="4"/>
-        <v>15</v>
-      </c>
-      <c r="E261" s="9">
-        <v>3</v>
-      </c>
-      <c r="F261" s="9">
-        <v>6</v>
-      </c>
-      <c r="G261" s="9">
-        <f>SUM(K251:K261)</f>
-        <v>165</v>
-      </c>
-      <c r="H261" s="9">
-        <f>COUNTA(J251:J261)</f>
-        <v>11</v>
-      </c>
-      <c r="J261" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="K261" s="9">
-        <v>15</v>
-      </c>
+      <c r="C261" s="10"/>
+      <c r="D261" s="9"/>
+      <c r="E261" s="9"/>
+      <c r="F261" s="9"/>
+      <c r="G261" s="9"/>
+      <c r="H261" s="9"/>
+      <c r="J261" s="11"/>
+      <c r="K261" s="11"/>
     </row>
     <row r="306" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C306" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D306" s="2"/>
       <c r="E306" s="2"/>
@@ -13020,34 +13218,30 @@
         <v>0</v>
       </c>
       <c r="D307" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E307" s="5" t="s">
         <v>1</v>
       </c>
       <c r="F307" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G307" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H307" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H307" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J307" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="K307" s="5" t="s">
-        <v>25</v>
-      </c>
+      <c r="J307" s="7"/>
+      <c r="K307" s="7"/>
     </row>
     <row r="308" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C308" s="10">
-        <v>44250</v>
+        <v>44265</v>
       </c>
       <c r="D308" s="9">
         <f>G308/H308</f>
-        <v>15</v>
+        <v>0.91304347826086951</v>
       </c>
       <c r="E308" s="9">
         <v>3</v>
@@ -13056,27 +13250,21 @@
         <v>6</v>
       </c>
       <c r="G308" s="9">
-        <f>SUM(K308:K318)</f>
-        <v>165</v>
+        <v>21</v>
       </c>
       <c r="H308" s="9">
-        <f>COUNTA(J308:J318)</f>
-        <v>11</v>
-      </c>
-      <c r="J308" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="K308" s="9">
-        <v>15</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="J308" s="11"/>
+      <c r="K308" s="11"/>
     </row>
     <row r="309" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C309" s="10">
-        <v>44251</v>
+        <v>44270</v>
       </c>
       <c r="D309" s="9">
         <f t="shared" ref="D309:D312" si="5">G309/H309</f>
-        <v>15</v>
+        <v>1.0689655172413792</v>
       </c>
       <c r="E309" s="9">
         <v>3</v>
@@ -13085,27 +13273,21 @@
         <v>6</v>
       </c>
       <c r="G309" s="9">
-        <f>SUM(K308:K318)</f>
-        <v>165</v>
+        <v>31</v>
       </c>
       <c r="H309" s="9">
-        <f>COUNTA(J308:J318)</f>
-        <v>11</v>
-      </c>
-      <c r="J309" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="K309" s="9">
-        <v>15</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="J309" s="11"/>
+      <c r="K309" s="11"/>
     </row>
     <row r="310" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C310" s="10">
-        <v>44252</v>
+        <v>44275</v>
       </c>
       <c r="D310" s="9">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="E310" s="9">
         <v>3</v>
@@ -13114,27 +13296,22 @@
         <v>6</v>
       </c>
       <c r="G310" s="9">
-        <f>SUM(K308:K318)</f>
-        <v>165</v>
+        <v>44</v>
       </c>
       <c r="H310" s="9">
-        <f>COUNTA(J308:J318)</f>
-        <v>11</v>
-      </c>
-      <c r="J310" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="K310" s="9">
-        <v>15</v>
-      </c>
+        <f>29+19</f>
+        <v>48</v>
+      </c>
+      <c r="J310" s="11"/>
+      <c r="K310" s="11"/>
     </row>
     <row r="311" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C311" s="10">
-        <v>44253</v>
+        <v>44280</v>
       </c>
       <c r="D311" s="9">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>1.4098360655737705</v>
       </c>
       <c r="E311" s="9">
         <v>3</v>
@@ -13143,27 +13320,23 @@
         <v>6</v>
       </c>
       <c r="G311" s="9">
-        <f>SUM(K308:K318)</f>
-        <v>165</v>
+        <f>86</f>
+        <v>86</v>
       </c>
       <c r="H311" s="9">
-        <f>COUNTA(J308:J318)</f>
-        <v>11</v>
-      </c>
-      <c r="J311" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="K311" s="9">
-        <v>15</v>
-      </c>
+        <f>48+13</f>
+        <v>61</v>
+      </c>
+      <c r="J311" s="11"/>
+      <c r="K311" s="11"/>
     </row>
     <row r="312" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C312" s="10">
-        <v>44254</v>
+        <v>44285</v>
       </c>
       <c r="D312" s="9">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>1.4098360655737705</v>
       </c>
       <c r="E312" s="9">
         <v>3</v>
@@ -13172,27 +13345,22 @@
         <v>6</v>
       </c>
       <c r="G312" s="9">
-        <f>SUM(K308:K318)</f>
-        <v>165</v>
+        <f>86</f>
+        <v>86</v>
       </c>
       <c r="H312" s="9">
-        <f>COUNTA(J308:J318)</f>
-        <v>11</v>
-      </c>
-      <c r="J312" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="K312" s="9">
-        <v>15</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="J312" s="11"/>
+      <c r="K312" s="11"/>
     </row>
     <row r="313" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C313" s="10">
-        <v>44255</v>
+        <v>44290</v>
       </c>
       <c r="D313" s="9">
         <f>G313/H313</f>
-        <v>15</v>
+        <v>1.4098360655737705</v>
       </c>
       <c r="E313" s="9">
         <v>3</v>
@@ -13201,27 +13369,22 @@
         <v>6</v>
       </c>
       <c r="G313" s="9">
-        <f>SUM(K308:K318)</f>
-        <v>165</v>
+        <f>86</f>
+        <v>86</v>
       </c>
       <c r="H313" s="9">
-        <f>COUNTA(J308:J318)</f>
-        <v>11</v>
-      </c>
-      <c r="J313" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="K313" s="9">
-        <v>15</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="J313" s="11"/>
+      <c r="K313" s="11"/>
     </row>
     <row r="314" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C314" s="10">
-        <v>44256</v>
+        <v>44295</v>
       </c>
       <c r="D314" s="9">
         <f t="shared" ref="D314:D318" si="6">G314/H314</f>
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="E314" s="9">
         <v>3</v>
@@ -13230,27 +13393,21 @@
         <v>6</v>
       </c>
       <c r="G314" s="9">
-        <f>SUM(K308:K318)</f>
-        <v>165</v>
+        <v>96</v>
       </c>
       <c r="H314" s="9">
-        <f>COUNTA(J308:J318)</f>
-        <v>11</v>
-      </c>
-      <c r="J314" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="K314" s="9">
-        <v>15</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="J314" s="11"/>
+      <c r="K314" s="11"/>
     </row>
     <row r="315" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C315" s="10">
-        <v>44257</v>
+        <v>44300</v>
       </c>
       <c r="D315" s="9">
         <f t="shared" si="6"/>
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="E315" s="9">
         <v>3</v>
@@ -13259,110 +13416,47 @@
         <v>6</v>
       </c>
       <c r="G315" s="9">
-        <f>SUM(K308:K318)</f>
-        <v>165</v>
+        <v>96</v>
       </c>
       <c r="H315" s="9">
-        <f>COUNTA(J308:J318)</f>
-        <v>11</v>
-      </c>
-      <c r="J315" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="K315" s="9">
-        <v>15</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="J315" s="11"/>
+      <c r="K315" s="11"/>
     </row>
     <row r="316" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C316" s="10">
-        <v>44258</v>
-      </c>
-      <c r="D316" s="9">
-        <f t="shared" si="6"/>
-        <v>15</v>
-      </c>
-      <c r="E316" s="9">
-        <v>3</v>
-      </c>
-      <c r="F316" s="9">
-        <v>6</v>
-      </c>
-      <c r="G316" s="9">
-        <f>SUM(K308:K318)</f>
-        <v>165</v>
-      </c>
-      <c r="H316" s="9">
-        <f>COUNTA(J308:J318)</f>
-        <v>11</v>
-      </c>
-      <c r="J316" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="K316" s="9">
-        <v>15</v>
-      </c>
+      <c r="C316" s="10"/>
+      <c r="D316" s="9"/>
+      <c r="E316" s="9"/>
+      <c r="F316" s="9"/>
+      <c r="G316" s="9"/>
+      <c r="H316" s="9"/>
+      <c r="J316" s="11"/>
+      <c r="K316" s="11"/>
     </row>
     <row r="317" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C317" s="10">
-        <v>44259</v>
-      </c>
-      <c r="D317" s="9">
-        <f t="shared" si="6"/>
-        <v>15</v>
-      </c>
-      <c r="E317" s="9">
-        <v>3</v>
-      </c>
-      <c r="F317" s="9">
-        <v>6</v>
-      </c>
-      <c r="G317" s="9">
-        <f>SUM(K308:K318)</f>
-        <v>165</v>
-      </c>
-      <c r="H317" s="9">
-        <f>COUNTA(J308:J318)</f>
-        <v>11</v>
-      </c>
-      <c r="J317" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="K317" s="9">
-        <v>15</v>
-      </c>
+      <c r="C317" s="10"/>
+      <c r="D317" s="9"/>
+      <c r="E317" s="9"/>
+      <c r="F317" s="9"/>
+      <c r="G317" s="9"/>
+      <c r="H317" s="9"/>
+      <c r="J317" s="11"/>
+      <c r="K317" s="11"/>
     </row>
     <row r="318" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C318" s="10">
-        <v>44260</v>
-      </c>
-      <c r="D318" s="9">
-        <f t="shared" si="6"/>
-        <v>15</v>
-      </c>
-      <c r="E318" s="9">
-        <v>3</v>
-      </c>
-      <c r="F318" s="9">
-        <v>6</v>
-      </c>
-      <c r="G318" s="9">
-        <f>SUM(K308:K318)</f>
-        <v>165</v>
-      </c>
-      <c r="H318" s="9">
-        <f>COUNTA(J308:J318)</f>
-        <v>11</v>
-      </c>
-      <c r="J318" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="K318" s="9">
-        <v>15</v>
-      </c>
+      <c r="C318" s="10"/>
+      <c r="D318" s="9"/>
+      <c r="E318" s="9"/>
+      <c r="F318" s="9"/>
+      <c r="G318" s="9"/>
+      <c r="H318" s="9"/>
+      <c r="J318" s="11"/>
+      <c r="K318" s="11"/>
     </row>
     <row r="367" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C367" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D367" s="2"/>
       <c r="E367" s="2"/>
@@ -13372,13 +13466,13 @@
         <v>0</v>
       </c>
       <c r="D368" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E368" s="5" t="s">
         <v>1</v>
       </c>
       <c r="F368" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="369" spans="3:6" x14ac:dyDescent="0.3">

</xml_diff>